<commit_message>
- removed C8 and C10 from all variants as tests showed that without these the SPI can be clocked a little faster
</commit_message>
<xml_diff>
--- a/L-D5019-01-04/Project Outputs/L-D5019-01-04.xlsx
+++ b/L-D5019-01-04/Project Outputs/L-D5019-01-04.xlsx
@@ -68,7 +68,7 @@
     <t xml:space="preserve">CAPC_0805</t>
   </si>
   <si>
-    <t xml:space="preserve">C2, C3, C4, C5, C8, C10</t>
+    <t xml:space="preserve">C2, C3, C4, C5</t>
   </si>
   <si>
     <t xml:space="preserve">22p</t>
@@ -317,6 +317,7 @@
       <sz val="10"/>
       <name val="Tahoma"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -523,7 +524,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -531,7 +532,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="61.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.96"/>
@@ -595,7 +596,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>14</v>

</xml_diff>